<commit_message>
Added four course exercises.
</commit_message>
<xml_diff>
--- a/resources/Part_3_Statistics/S15_L74/2.3.Categorical-variables.Visualization-techniques-exercise.xlsx
+++ b/resources/Part_3_Statistics/S15_L74/2.3.Categorical-variables.Visualization-techniques-exercise.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19695" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Frequency distribution table" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,18 @@
     <sheet name="Pie chart" sheetId="7" r:id="rId3"/>
     <sheet name="Pareto diagram" sheetId="12" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Frequency distribution table'!$F$14</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Frequency distribution table'!$G$13:$I$13</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Frequency distribution table'!$G$14:$I$14</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Frequency distribution table'!$F$14</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Frequency distribution table'!$G$13:$I$13</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Frequency distribution table'!$G$14:$I$14</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Frequency distribution table'!$F$14</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Frequency distribution table'!$G$13:$I$13</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Frequency distribution table'!$G$14:$I$14</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Background</t>
   </si>
@@ -89,6 +100,21 @@
   </si>
   <si>
     <t>You have sold 12,327 ice creams in New York; 17,129 in LA and 19,923 in San Francisco.</t>
+  </si>
+  <si>
+    <t>N.Y.</t>
+  </si>
+  <si>
+    <t>L.A.</t>
+  </si>
+  <si>
+    <t>S.F.</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Ice cream sold</t>
   </si>
 </sst>
 </file>
@@ -179,7 +205,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -196,11 +222,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,6 +247,2333 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Frequency distribution table'!$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ice cream sold</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Frequency distribution table'!$G$13:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>N.Y.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>L.A.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S.F.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Frequency distribution table'!$G$14:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19933</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7015-4EE1-B9DA-45C35DC2081F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1778557456"/>
+        <c:axId val="1778559952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1778557456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1778559952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1778559952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1778557456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Frequency distribution table'!$F$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ice cream sold</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-EA11-41D5-BF3C-0E913983CC6A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EA11-41D5-BF3C-0E913983CC6A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-EA11-41D5-BF3C-0E913983CC6A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Frequency distribution table'!$G$13:$I$13</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>N.Y.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>L.A.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S.F.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Frequency distribution table'!$G$14:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19933</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-EA11-41D5-BF3C-0E913983CC6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{06E4C936-156E-4478-99C4-27106A647425}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v>Ice cream sold</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:aggregation/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{C4E0DCE8-DBD6-484E-8333-A68CB6B07BC6}">
+          <cx:axisId val="2"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <cx:printSettings>
+    <cx:headerFooter alignWithMargins="1" differentOddEven="0" differentFirst="0"/>
+    <cx:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <cx:pageSetup paperSize="1" firstPageNumber="1" orientation="default" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  </cx:printSettings>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Gráfico 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,35 +2839,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="12.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,7 +2878,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
@@ -529,7 +2887,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
@@ -538,35 +2896,58 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D9" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+      <c r="F13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+      <c r="F14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="3">
+        <v>12327</v>
+      </c>
+      <c r="H14" s="3">
+        <v>17129</v>
+      </c>
+      <c r="I14" s="3">
+        <v>19933</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
@@ -574,7 +2955,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
@@ -582,7 +2963,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
@@ -664,28 +3045,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="12.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +3077,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -709,7 +3092,7 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -745,7 +3128,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
@@ -763,7 +3146,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -781,7 +3164,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
@@ -800,7 +3183,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
@@ -819,7 +3202,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
@@ -1189,6 +3572,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1196,29 +3580,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +3613,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1236,7 +3622,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1244,7 +3630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
@@ -1262,7 +3648,7 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="7"/>
@@ -1280,7 +3666,7 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -1299,7 +3685,7 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
@@ -1318,7 +3704,7 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
@@ -1337,7 +3723,7 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
@@ -1356,7 +3742,7 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:17" ht="12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
@@ -1526,6 +3912,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1533,29 +3920,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1563,7 +3952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1571,7 +3960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +3968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1587,7 +3976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1596,12 +3985,12 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="7"/>
@@ -1613,7 +4002,7 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
       <c r="D11" s="7"/>
@@ -1625,7 +4014,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="11"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1637,7 +4026,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
       <c r="D13" s="9"/>
@@ -1649,7 +4038,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
       <c r="D14" s="9"/>
@@ -1661,7 +4050,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
       <c r="D15" s="9"/>
@@ -1673,7 +4062,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:11" ht="12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
       <c r="D16" s="9"/>
@@ -1709,7 +4098,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="2:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1760,5 +4149,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>